<commit_message>
Details Added In Config.xlsx
</commit_message>
<xml_diff>
--- a/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
+++ b/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BNS\UiPath\UP_Template_BNS_REFramework\UP_Template_BNS_REFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BNS\UiPath\UP_Process_Performer_UnsecuredVendorA50ROO\UP_Process_Performer_UnsecuredVendorA50ROO\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA3C075-FE22-4B06-ADC6-E98304AFC6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077D4DA2-8A35-42A3-807B-5DEA6BB4C9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Read Config Settings Json string from Asset 'RobotConfig'.</t>
+  </si>
+  <si>
+    <t>RobotConfigPerformer</t>
+  </si>
+  <si>
+    <t>Canadian Banking/Canadian Banking/Canadian Banking Operations/Canada Collections/Back End Collections/437 - Unsecured Vendor (A50 ROO) 2.0</t>
   </si>
 </sst>
 </file>
@@ -513,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -663,7 +669,7 @@
         <v>32</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>437</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -679,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -732,7 +738,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Added config settings for each collectionhighway IDs.
</commit_message>
<xml_diff>
--- a/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
+++ b/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Drive\_UIPath\GIT\UP_Process_Performer_UnsecuredVendorA50ROO\UP_Process_Performer_UnsecuredVendorA50ROO\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA8B761-D9B2-4B05-B02A-70672A4EEA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BED45B-741D-4A34-99B9-49568C785ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -138,6 +138,21 @@
   </si>
   <si>
     <t>DHStatus</t>
+  </si>
+  <si>
+    <t>PwUpdated_BNSTESTERB</t>
+  </si>
+  <si>
+    <t>PwUpdated_BNSTESTERC</t>
+  </si>
+  <si>
+    <t>TestData_ProductID</t>
+  </si>
+  <si>
+    <t>TestData_ProductType</t>
+  </si>
+  <si>
+    <t>TestData_StateCode</t>
   </si>
 </sst>
 </file>
@@ -754,11 +769,46 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updates to password reset
</commit_message>
<xml_diff>
--- a/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
+++ b/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Drive\_UIPath\GIT\UP_Process_Performer_UnsecuredVendorA50ROO\UP_Process_Performer_UnsecuredVendorA50ROO\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BED45B-741D-4A34-99B9-49568C785ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABCE8E5-573D-4095-8AF4-56CCAAE0BA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,12 +140,6 @@
     <t>DHStatus</t>
   </si>
   <si>
-    <t>PwUpdated_BNSTESTERB</t>
-  </si>
-  <si>
-    <t>PwUpdated_BNSTESTERC</t>
-  </si>
-  <si>
     <t>TestData_ProductID</t>
   </si>
   <si>
@@ -153,6 +147,12 @@
   </si>
   <si>
     <t>TestData_StateCode</t>
+  </si>
+  <si>
+    <t>PwdUpdated_BNSTESTERB</t>
+  </si>
+  <si>
+    <t>PwdUpdated_BNSTESTERC</t>
   </si>
 </sst>
 </file>
@@ -771,42 +771,42 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
delete the storage bucket automations from process flow
</commit_message>
<xml_diff>
--- a/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
+++ b/UP_Process_Performer_UnsecuredVendorA50ROO/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Drive\_UIPath\GIT\UP_Process_Performer_UnsecuredVendorA50ROO\UP_Process_Performer_UnsecuredVendorA50ROO\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BNS\UIPath\UP_Process_Performer_UnsecuredVendorA50ROO\UP_Process_Performer_UnsecuredVendorA50ROO\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3283584-2B98-4AAC-AB76-4D031D61EAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAF603C-70C7-4F83-A859-D5E6C9365966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -138,12 +138,6 @@
   </si>
   <si>
     <t>DHStatus</t>
-  </si>
-  <si>
-    <t>PwdUpdated_BNSTESTERB</t>
-  </si>
-  <si>
-    <t>PwdUpdated_BNSTESTERC</t>
   </si>
 </sst>
 </file>
@@ -528,17 +522,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18">
+    <row r="1" spans="1:26" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="28.8">
+    <row r="9" spans="1:26" ht="45">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -660,7 +654,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="28.8">
+    <row r="10" spans="1:26" ht="30">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -692,14 +686,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -760,22 +756,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>